<commit_message>
Updated chemical id mapping
</commit_message>
<xml_diff>
--- a/data/dataSchemas/processingPipelineSchema.xlsx
+++ b/data/dataSchemas/processingPipelineSchema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/data/dataSchemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{C2D895B9-4381-46C9-BE1A-BB38FE0B8351}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{22429932-CDB4-42B3-9C55-97D351353BC6}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{C2D895B9-4381-46C9-BE1A-BB38FE0B8351}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8D8419B3-6EFF-4FF7-BBC3-26CF0AB1052A}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="12150" windowHeight="20835" xr2:uid="{3244EBFB-4E91-45FC-B66B-30D163E3937A}"/>
+    <workbookView xWindow="6390" yWindow="1170" windowWidth="12150" windowHeight="14430" xr2:uid="{3244EBFB-4E91-45FC-B66B-30D163E3937A}"/>
   </bookViews>
   <sheets>
     <sheet name="environmentalSample" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>SampleNumber</t>
   </si>
@@ -186,6 +186,93 @@
   </si>
   <si>
     <t xml:space="preserve">sometimes starts with capital c </t>
+  </si>
+  <si>
+    <t>Date sampled</t>
+  </si>
+  <si>
+    <t>Sample Number</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>Location Name</t>
+  </si>
+  <si>
+    <t>Location Description</t>
+  </si>
+  <si>
+    <t>Alternate Name</t>
+  </si>
+  <si>
+    <t>Chemical ID</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>ZF Lims Id</t>
+  </si>
+  <si>
+    <t>CAS Number</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>Concentration Unity</t>
+  </si>
+  <si>
+    <t>Sample Concentration</t>
+  </si>
+  <si>
+    <t>Sample Molar Concentration</t>
+  </si>
+  <si>
+    <t>Environmental Concentration</t>
+  </si>
+  <si>
+    <t>Environmental Concentration Unit</t>
+  </si>
+  <si>
+    <t>Environmental Molar Concentration</t>
+  </si>
+  <si>
+    <t>Environmental Molar Concentration Unit</t>
+  </si>
+  <si>
+    <t>Sample Molar Concentration Unit</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Parent Sample Number</t>
+  </si>
+  <si>
+    <t>Child Sample Number</t>
   </si>
 </sst>
 </file>
@@ -557,14 +644,14 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
@@ -593,11 +680,20 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -606,138 +702,265 @@
       <c r="B4" t="s">
         <v>46</v>
       </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>